<commit_message>
Test XLS now in Git
</commit_message>
<xml_diff>
--- a/src/test/resources/beitrag.xlsx
+++ b/src/test/resources/beitrag.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/palmherby/Entwickeln/netBeansProjects/ExcelDemo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/palmherby/Entwickeln/netBeansProjects/ExcelDemo/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Beitragserhöhung</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>vnr</t>
   </si>
@@ -45,6 +42,15 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>Standard</t>
+  </si>
+  <si>
+    <t>1234.5</t>
+  </si>
+  <si>
+    <t>Beitragsaenderung</t>
   </si>
 </sst>
 </file>
@@ -80,8 +86,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Stand." xfId="0" builtinId="0"/>
@@ -361,9 +368,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -372,32 +377,44 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>5</v>
-      </c>
-      <c r="F2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>70123456</v>
+      </c>
+      <c r="B3" s="1">
+        <v>42705</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>